<commit_message>
params updated (treatment rates)
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.jemmett\dev\R\active_projects\723_mh_covid_surge_modelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A30057-9607-43FD-95D4-51D6677EABFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF64233-CDB0-4E4F-9CB2-7082DA32CCF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{F50B436A-7669-4109-9972-A64F78759D89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F50B436A-7669-4109-9972-A64F78759D89}"/>
   </bookViews>
   <sheets>
     <sheet name="groups" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="60">
   <si>
     <t>General population</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Follow the curve</t>
+  </si>
+  <si>
+    <t>Psychosis</t>
   </si>
 </sst>
 </file>
@@ -258,11 +261,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,9 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2794AB8-A2FA-4898-8B2A-2A83645A0C40}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -838,9 +840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FA8F3A-40A9-4BA2-90D8-EC2D921A3DDC}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1499,9 +1499,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B041FEA-7504-47C5-AC33-EE86F088EA46}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1534,7 +1534,7 @@
         <v>0.2</v>
       </c>
       <c r="D2">
-        <v>0.62</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1548,7 +1548,7 @@
         <v>0.05</v>
       </c>
       <c r="D3">
-        <v>0.62</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1562,7 +1562,7 @@
         <v>0.6</v>
       </c>
       <c r="D4">
-        <v>0.62</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
         <v>0.15</v>
       </c>
       <c r="D5">
-        <v>0.62</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1590,7 +1590,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.62</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1604,7 +1604,7 @@
         <v>0.13513513513513514</v>
       </c>
       <c r="D7">
-        <v>0.62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1618,7 +1618,7 @@
         <v>0.27027027027027029</v>
       </c>
       <c r="D8">
-        <v>0.62</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1632,7 +1632,7 @@
         <v>0.27027027027027029</v>
       </c>
       <c r="D9">
-        <v>0.62</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
         <v>0.10810810810810811</v>
       </c>
       <c r="D10">
-        <v>0.62</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
         <v>0.21621621621621623</v>
       </c>
       <c r="D11">
-        <v>0.62</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1674,7 +1674,7 @@
         <v>0.43749999999999994</v>
       </c>
       <c r="D12">
-        <v>0.62</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1688,7 +1688,7 @@
         <v>0.25</v>
       </c>
       <c r="D13">
-        <v>0.62</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1702,7 +1702,7 @@
         <v>0.3125</v>
       </c>
       <c r="D14">
-        <v>0.62</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1716,7 +1716,7 @@
         <v>8.5714285714285701E-2</v>
       </c>
       <c r="D15">
-        <v>0.62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1730,7 +1730,7 @@
         <v>0.22857142857142856</v>
       </c>
       <c r="D16">
-        <v>0.62</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1744,7 +1744,7 @@
         <v>0.22857142857142856</v>
       </c>
       <c r="D17">
-        <v>0.62</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1758,7 +1758,7 @@
         <v>0.22857142857142856</v>
       </c>
       <c r="D18">
-        <v>0.62</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1772,7 +1772,7 @@
         <v>0.22857142857142856</v>
       </c>
       <c r="D19">
-        <v>0.62</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1786,7 +1786,7 @@
         <v>5.2631578947368425E-2</v>
       </c>
       <c r="D20">
-        <v>0.62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1800,7 +1800,7 @@
         <v>0.2105263157894737</v>
       </c>
       <c r="D21">
-        <v>0.62</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1814,7 +1814,7 @@
         <v>0.2105263157894737</v>
       </c>
       <c r="D22">
-        <v>0.62</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1828,7 +1828,7 @@
         <v>0.10526315789473685</v>
       </c>
       <c r="D23">
-        <v>0.62</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1842,7 +1842,7 @@
         <v>0.4210526315789474</v>
       </c>
       <c r="D24">
-        <v>0.62</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1856,7 +1856,7 @@
         <v>0.8</v>
       </c>
       <c r="D25">
-        <v>0.62</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1870,7 +1870,7 @@
         <v>0.2</v>
       </c>
       <c r="D26">
-        <v>0.62</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1884,7 +1884,7 @@
         <v>8.2644628099173556E-3</v>
       </c>
       <c r="D27">
-        <v>0.62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1898,7 +1898,7 @@
         <v>8.2644628099173556E-2</v>
       </c>
       <c r="D28">
-        <v>0.62</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1912,7 +1912,7 @@
         <v>4.1322314049586778E-2</v>
       </c>
       <c r="D29">
-        <v>0.62</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1926,7 +1926,7 @@
         <v>0.24793388429752067</v>
       </c>
       <c r="D30">
-        <v>0.62</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1940,7 +1940,7 @@
         <v>0.57851239669421484</v>
       </c>
       <c r="D31">
-        <v>0.62</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1954,161 +1954,161 @@
         <v>4.1322314049586778E-2</v>
       </c>
       <c r="D32">
-        <v>0.62</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>10</v>
+      <c r="A33" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B33" t="s">
         <v>40</v>
       </c>
       <c r="C33">
-        <v>0.11538461538461538</v>
+        <v>0.11764705882352942</v>
       </c>
       <c r="D33">
-        <v>0.62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>10</v>
+      <c r="A34" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C34">
-        <v>0.15384615384615385</v>
+        <v>0.11764705882352942</v>
       </c>
       <c r="D34">
-        <v>0.62</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>10</v>
+      <c r="A35" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C35">
-        <v>0.30769230769230771</v>
+        <v>0.29411764705882354</v>
       </c>
       <c r="D35">
-        <v>0.62</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>10</v>
+      <c r="A36" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C36">
-        <v>0.11538461538461538</v>
+        <v>0.23529411764705885</v>
       </c>
       <c r="D36">
-        <v>0.62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>10</v>
+      <c r="A37" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C37">
-        <v>0.30769230769230771</v>
+        <v>0.11764705882352942</v>
       </c>
       <c r="D37">
-        <v>0.62</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>5</v>
+      <c r="A38" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C38">
-        <v>0.13636363636363635</v>
+        <v>0.11764705882352942</v>
       </c>
       <c r="D38">
-        <v>0.62</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C39">
-        <v>0.13636363636363635</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="D39">
-        <v>0.62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C40">
-        <v>4.5454545454545456E-2</v>
+        <v>0.11538461538461538</v>
       </c>
       <c r="D40">
-        <v>0.62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C41">
-        <v>0.13636363636363635</v>
+        <v>0.30769230769230771</v>
       </c>
       <c r="D41">
-        <v>0.62</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C42">
-        <v>0.36363636363636365</v>
+        <v>0.11538461538461538</v>
       </c>
       <c r="D42">
-        <v>0.62</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C43">
-        <v>9.0909090909090912E-2</v>
+        <v>0.30769230769230771</v>
       </c>
       <c r="D43">
-        <v>0.62</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2116,181 +2116,181 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C44">
-        <v>9.0909090909090912E-2</v>
+        <v>0.13636363636363635</v>
       </c>
       <c r="D44">
-        <v>0.62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C45">
-        <v>0.24242424242424246</v>
+        <v>0.13636363636363635</v>
       </c>
       <c r="D45">
-        <v>0.62</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B46" t="s">
         <v>38</v>
       </c>
       <c r="C46">
-        <v>0.21212121212121213</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="D46">
-        <v>0.62</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C47">
-        <v>0.12121212121212123</v>
+        <v>0.13636363636363635</v>
       </c>
       <c r="D47">
-        <v>0.62</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="D48">
-        <v>0.62</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B49" t="s">
         <v>37</v>
       </c>
       <c r="C49">
-        <v>0.21212121212121213</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="D49">
-        <v>0.62</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B50" t="s">
         <v>43</v>
       </c>
       <c r="C50">
-        <v>0.21212121212121213</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="D50">
-        <v>0.62</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B51" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C51">
-        <v>0.3174603174603175</v>
+        <v>0.24242424242424246</v>
       </c>
       <c r="D51">
-        <v>0.62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B52" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C52">
-        <v>9.5238095238095247E-2</v>
+        <v>0.21212121212121213</v>
       </c>
       <c r="D52">
-        <v>0.62</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C53">
-        <v>0.22222222222222224</v>
+        <v>0.12121212121212123</v>
       </c>
       <c r="D53">
-        <v>0.62</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C54">
-        <v>1.5873015873015876E-2</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>0.62</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C55">
-        <v>9.5238095238095247E-2</v>
+        <v>0.21212121212121213</v>
       </c>
       <c r="D55">
-        <v>0.62</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C56">
-        <v>0.15873015873015875</v>
+        <v>0.21212121212121213</v>
       </c>
       <c r="D56">
-        <v>0.62</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2298,97 +2298,97 @@
         <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C57">
-        <v>9.5238095238095247E-2</v>
+        <v>0.3174603174603175</v>
       </c>
       <c r="D57">
-        <v>0.62</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C58">
-        <v>0.1</v>
+        <v>9.5238095238095247E-2</v>
       </c>
       <c r="D58">
-        <v>0.62</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C59">
-        <v>0.1</v>
+        <v>0.22222222222222224</v>
       </c>
       <c r="D59">
-        <v>0.62</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C60">
-        <v>0.125</v>
+        <v>1.5873015873015876E-2</v>
       </c>
       <c r="D60">
-        <v>0.62</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C61">
-        <v>0.125</v>
+        <v>9.5238095238095247E-2</v>
       </c>
       <c r="D61">
-        <v>0.62</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C62">
-        <v>0.2</v>
+        <v>0.15873015873015875</v>
       </c>
       <c r="D62">
-        <v>0.62</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C63">
-        <v>0.17499999999999999</v>
+        <v>9.5238095238095247E-2</v>
       </c>
       <c r="D63">
-        <v>0.62</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2396,13 +2396,97 @@
         <v>4</v>
       </c>
       <c r="B64" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64">
+        <v>0.1</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65">
+        <v>0.1</v>
+      </c>
+      <c r="D65">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" t="s">
+        <v>38</v>
+      </c>
+      <c r="C66">
+        <v>0.125</v>
+      </c>
+      <c r="D66">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67">
+        <v>0.125</v>
+      </c>
+      <c r="D67">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" t="s">
+        <v>42</v>
+      </c>
+      <c r="C68">
+        <v>0.2</v>
+      </c>
+      <c r="D68">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" t="s">
+        <v>37</v>
+      </c>
+      <c r="C69">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="D69">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" t="s">
         <v>43</v>
       </c>
-      <c r="C64">
+      <c r="C70">
         <v>0.17499999999999999</v>
       </c>
-      <c r="D64">
-        <v>0.62</v>
+      <c r="D70">
+        <v>0.28999999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2415,9 +2499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCCD7C2-90E2-4A03-AE81-9931C4408294}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2750,21 +2832,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F00E7D3C5223B647BCF0704F4FD63FF8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="274554e3832af7cc9064f5d6743782b1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c3b4031e-841f-46f6-bede-a60d28c4ce79" xmlns:ns3="25f82bdf-59aa-449e-b461-28a7236b0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2c96c06903633a0219cb8332eecd029" ns2:_="" ns3:_="">
     <xsd:import namespace="c3b4031e-841f-46f6-bede-a60d28c4ce79"/>
@@ -2981,32 +3048,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23E7D15A-7770-4D3B-91AE-A46500598E63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="60b7aa15-f80a-4fdd-839c-f4bbc2217594"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="af42b274-6a0d-4eb8-b3e5-ec8ba19bd91a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68A1C96F-6EFB-4028-BCE1-ECC515F0B18C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E8936A6-10D5-4CB1-A985-45E67CE71791}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3023,4 +3080,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68A1C96F-6EFB-4028-BCE1-ECC515F0B18C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23E7D15A-7770-4D3B-91AE-A46500598E63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="60b7aa15-f80a-4fdd-839c-f4bbc2217594"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="af42b274-6a0d-4eb8-b3e5-ec8ba19bd91a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
moves curves into params.xlsx/params.json
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.jemmett\dev\R\active_projects\723_mh_covid_surge_modelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF64233-CDB0-4E4F-9CB2-7082DA32CCF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3526AACB-95B8-4088-880C-82EBBAEA7594}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F50B436A-7669-4109-9972-A64F78759D89}"/>
   </bookViews>
   <sheets>
-    <sheet name="groups" sheetId="5" r:id="rId1"/>
-    <sheet name="g2c" sheetId="1" r:id="rId2"/>
-    <sheet name="c2t" sheetId="2" r:id="rId3"/>
-    <sheet name="treatments" sheetId="3" r:id="rId4"/>
+    <sheet name="curves" sheetId="6" r:id="rId1"/>
+    <sheet name="groups" sheetId="5" r:id="rId2"/>
+    <sheet name="g2c" sheetId="1" r:id="rId3"/>
+    <sheet name="c2t" sheetId="2" r:id="rId4"/>
+    <sheet name="treatments" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="64">
   <si>
     <t>General population</t>
   </si>
@@ -216,6 +217,18 @@
   </si>
   <si>
     <t>Psychosis</t>
+  </si>
+  <si>
+    <t>Sudden shock</t>
+  </si>
+  <si>
+    <t>Shallow mid-term</t>
+  </si>
+  <si>
+    <t>Sustained impact</t>
+  </si>
+  <si>
+    <t>month</t>
   </si>
 </sst>
 </file>
@@ -580,10 +593,455 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78CFF802-C4B0-4A2E-AEB8-42306206B753}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>6.1199999999999997E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="D3">
+        <v>7.6E-3</v>
+      </c>
+      <c r="E3">
+        <v>1.18E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.12239999999999999</v>
+      </c>
+      <c r="C4">
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.52E-2</v>
+      </c>
+      <c r="E4">
+        <v>2.3400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.24490000000000001</v>
+      </c>
+      <c r="C5">
+        <v>4.7500000000000001E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>3.7400000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.2041</v>
+      </c>
+      <c r="C6">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="D6">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="E6">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.1633</v>
+      </c>
+      <c r="C7">
+        <v>0.1188</v>
+      </c>
+      <c r="D7">
+        <v>3.7900000000000003E-2</v>
+      </c>
+      <c r="E7">
+        <v>4.48E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.1206</v>
+      </c>
+      <c r="D8">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="E8">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C9">
+        <v>0.1069</v>
+      </c>
+      <c r="D9">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E9">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="C10">
+        <v>8.4099999999999994E-2</v>
+      </c>
+      <c r="D10">
+        <v>6.0600000000000001E-2</v>
+      </c>
+      <c r="E10">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="C11">
+        <v>7.22E-2</v>
+      </c>
+      <c r="D11">
+        <v>6.8199999999999997E-2</v>
+      </c>
+      <c r="E11">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="C12">
+        <v>5.9400000000000001E-2</v>
+      </c>
+      <c r="D12">
+        <v>7.5800000000000006E-2</v>
+      </c>
+      <c r="E12">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>4.87E-2</v>
+      </c>
+      <c r="D13">
+        <v>8.3199999999999996E-2</v>
+      </c>
+      <c r="E13">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="D14">
+        <v>8.3199999999999996E-2</v>
+      </c>
+      <c r="E14">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="D15">
+        <v>7.5800000000000006E-2</v>
+      </c>
+      <c r="E15">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="D16">
+        <v>6.8199999999999997E-2</v>
+      </c>
+      <c r="E16">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>2.4899999999999999E-2</v>
+      </c>
+      <c r="D17">
+        <v>6.0600000000000001E-2</v>
+      </c>
+      <c r="E17">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="D18">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E18">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1.78E-2</v>
+      </c>
+      <c r="D19">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="E19">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1.43E-2</v>
+      </c>
+      <c r="D20">
+        <v>3.7900000000000003E-2</v>
+      </c>
+      <c r="E20">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="D21">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="E21">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D22">
+        <v>2.2700000000000001E-2</v>
+      </c>
+      <c r="E22">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="D23">
+        <v>1.52E-2</v>
+      </c>
+      <c r="E23">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="D24">
+        <v>7.6E-3</v>
+      </c>
+      <c r="E24">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2794AB8-A2FA-4898-8B2A-2A83645A0C40}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -836,7 +1294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FA8F3A-40A9-4BA2-90D8-EC2D921A3DDC}">
   <dimension ref="A1:C58"/>
   <sheetViews>
@@ -1497,7 +1955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B041FEA-7504-47C5-AC33-EE86F088EA46}">
   <dimension ref="A1:D70"/>
   <sheetViews>
@@ -2495,7 +2953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCCD7C2-90E2-4A03-AE81-9931C4408294}">
   <dimension ref="A1:O18"/>
   <sheetViews>
@@ -2832,6 +3290,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F00E7D3C5223B647BCF0704F4FD63FF8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="274554e3832af7cc9064f5d6743782b1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c3b4031e-841f-46f6-bede-a60d28c4ce79" xmlns:ns3="25f82bdf-59aa-449e-b461-28a7236b0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2c96c06903633a0219cb8332eecd029" ns2:_="" ns3:_="">
     <xsd:import namespace="c3b4031e-841f-46f6-bede-a60d28c4ce79"/>
@@ -3048,7 +3512,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3057,13 +3521,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23E7D15A-7770-4D3B-91AE-A46500598E63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="60b7aa15-f80a-4fdd-839c-f4bbc2217594"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="af42b274-6a0d-4eb8-b3e5-ec8ba19bd91a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E8936A6-10D5-4CB1-A985-45E67CE71791}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3082,27 +3557,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68A1C96F-6EFB-4028-BCE1-ECC515F0B18C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23E7D15A-7770-4D3B-91AE-A46500598E63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="60b7aa15-f80a-4fdd-839c-f4bbc2217594"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="af42b274-6a0d-4eb8-b3e5-ec8ba19bd91a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updates parameters, replaces - with spaces
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.jemmett\dev\R\active_projects\723_mh_covid_surge_modelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3526AACB-95B8-4088-880C-82EBBAEA7594}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1120B57D-6888-4A01-86A4-81B790866A0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F50B436A-7669-4109-9972-A64F78759D89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{F50B436A-7669-4109-9972-A64F78759D89}"/>
   </bookViews>
   <sheets>
     <sheet name="curves" sheetId="6" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>Suicide/ideation</t>
   </si>
   <si>
-    <t>Self-harm</t>
-  </si>
-  <si>
     <t>Substance misuse</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>PTSD</t>
   </si>
   <si>
-    <t>Neurological symptom disorder (ADHD / Aspergers)</t>
-  </si>
-  <si>
     <t>Students FE &amp; HE</t>
   </si>
   <si>
@@ -87,12 +81,6 @@
     <t>Insomnia</t>
   </si>
   <si>
-    <t>Pre-existing LTC</t>
-  </si>
-  <si>
-    <t>Pre-existing SMI</t>
-  </si>
-  <si>
     <t>Newly unemployed</t>
   </si>
   <si>
@@ -102,9 +90,6 @@
     <t>Complicated grief</t>
   </si>
   <si>
-    <t>Pre-existing CMH illness</t>
-  </si>
-  <si>
     <t>Pregnant &amp; New Mothers</t>
   </si>
   <si>
@@ -114,9 +99,6 @@
     <t>Domestic abuse victims</t>
   </si>
   <si>
-    <t>Family of COVID-deceased</t>
-  </si>
-  <si>
     <t>pcnt</t>
   </si>
   <si>
@@ -222,13 +204,31 @@
     <t>Sudden shock</t>
   </si>
   <si>
-    <t>Shallow mid-term</t>
-  </si>
-  <si>
     <t>Sustained impact</t>
   </si>
   <si>
     <t>month</t>
+  </si>
+  <si>
+    <t>Self harm</t>
+  </si>
+  <si>
+    <t>Family of COVID deceased</t>
+  </si>
+  <si>
+    <t>Pre existing CMH illness</t>
+  </si>
+  <si>
+    <t>Pre existing LTC</t>
+  </si>
+  <si>
+    <t>Pre existing SMI</t>
+  </si>
+  <si>
+    <t>Shallow mid term</t>
+  </si>
+  <si>
+    <t>Neurological symptom disorder (ADHD/Aspergers)</t>
   </si>
 </sst>
 </file>
@@ -596,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78CFF802-C4B0-4A2E-AEB8-42306206B753}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -609,19 +609,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1053,24 +1053,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C2">
         <v>116654</v>
@@ -1081,10 +1081,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C3">
         <v>1956</v>
@@ -1095,10 +1095,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C4">
         <v>46105</v>
@@ -1109,10 +1109,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>4030</v>
@@ -1123,10 +1123,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>425</v>
@@ -1140,7 +1140,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>143087</v>
@@ -1151,10 +1151,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>16749</v>
@@ -1165,10 +1165,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C9">
         <v>85</v>
@@ -1179,10 +1179,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C10">
         <v>1683</v>
@@ -1193,10 +1193,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C11">
         <v>1097</v>
@@ -1207,10 +1207,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C12">
         <v>141371</v>
@@ -1221,10 +1221,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C13">
         <v>29902</v>
@@ -1235,10 +1235,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C14">
         <v>176849</v>
@@ -1249,10 +1249,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C15">
         <v>6408</v>
@@ -1263,10 +1263,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C16">
         <v>5621</v>
@@ -1277,10 +1277,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C17">
         <v>80575</v>
@@ -1298,7 +1298,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FA8F3A-40A9-4BA2-90D8-EC2D921A3DDC}">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1309,18 +1311,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1331,7 +1333,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1342,10 +1344,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2">
         <v>6.4000000000000003E-3</v>
@@ -1353,10 +1355,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
       </c>
       <c r="C5" s="2">
         <v>0.1</v>
@@ -1364,10 +1366,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2">
         <v>0.02</v>
@@ -1375,10 +1377,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2">
         <v>6.6666666669999999E-2</v>
@@ -1386,7 +1388,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -1397,10 +1399,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2">
         <v>0.21266666670000001</v>
@@ -1408,10 +1410,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2">
         <v>4.5666666669999995E-2</v>
@@ -1419,7 +1421,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -1430,7 +1432,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -1441,7 +1443,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -1452,10 +1454,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
@@ -1463,7 +1465,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -1474,10 +1476,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C16" s="2">
         <v>2.3333333330000001E-2</v>
@@ -1485,10 +1487,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
@@ -1496,7 +1498,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -1507,7 +1509,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
@@ -1518,10 +1520,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="2">
         <v>6.6666666669999999E-2</v>
@@ -1529,10 +1531,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2">
         <v>0.20333333329999997</v>
@@ -1540,7 +1542,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -1587,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C26" s="2">
         <v>1.666666667E-2</v>
@@ -1598,7 +1600,7 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C27" s="2">
         <v>2.7000000000000003E-2</v>
@@ -1609,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" s="2">
         <v>2.5666666669999998E-2</v>
@@ -1628,7 +1630,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -1639,7 +1641,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
         <v>2</v>
@@ -1650,10 +1652,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C32" s="2">
         <v>0.11333333330000001</v>
@@ -1661,10 +1663,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C33" s="2">
         <v>3.3333333329999999E-2</v>
@@ -1672,7 +1674,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
@@ -1683,7 +1685,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -1694,10 +1696,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" s="2">
         <v>6.6666666669999999E-2</v>
@@ -1705,10 +1707,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C37" s="2">
         <v>0.20333333329999997</v>
@@ -1716,7 +1718,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
         <v>4</v>
@@ -1727,10 +1729,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39" s="2">
         <v>6.6666666669999999E-2</v>
@@ -1738,7 +1740,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
@@ -1749,7 +1751,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
         <v>2</v>
@@ -1760,10 +1762,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C42" s="2">
         <v>0</v>
@@ -1771,10 +1773,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C43" s="2">
         <v>2.8888888889999999E-2</v>
@@ -1782,7 +1784,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
@@ -1793,7 +1795,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
@@ -1804,7 +1806,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B46" t="s">
         <v>2</v>
@@ -1815,10 +1817,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C47" s="2">
         <v>7.0000000000000007E-2</v>
@@ -1826,10 +1828,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C48" s="2">
         <v>3.3333333329999999E-2</v>
@@ -1837,7 +1839,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
@@ -1848,7 +1850,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B50" t="s">
         <v>2</v>
@@ -1859,10 +1861,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" s="2">
         <v>0.05</v>
@@ -1870,7 +1872,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
@@ -1881,10 +1883,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C53" s="2">
         <v>0.1</v>
@@ -1892,10 +1894,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C54" s="2">
         <v>8.3333333330000009E-2</v>
@@ -1903,7 +1905,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
         <v>3</v>
@@ -1914,7 +1916,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B56" t="s">
         <v>2</v>
@@ -1925,10 +1927,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C57" s="2">
         <v>0.03</v>
@@ -1936,10 +1938,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C58" s="2">
         <v>0</v>
@@ -1959,7 +1961,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B041FEA-7504-47C5-AC33-EE86F088EA46}">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1969,16 +1973,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1986,7 +1990,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>0.2</v>
@@ -2000,7 +2004,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>0.05</v>
@@ -2014,7 +2018,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>0.6</v>
@@ -2028,7 +2032,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>0.15</v>
@@ -2039,10 +2043,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2056,7 +2060,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C7">
         <v>0.13513513513513514</v>
@@ -2070,7 +2074,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>0.27027027027027029</v>
@@ -2084,7 +2088,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>0.27027027027027029</v>
@@ -2098,7 +2102,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>0.10810810810810811</v>
@@ -2112,7 +2116,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>0.21621621621621623</v>
@@ -2123,10 +2127,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>0.43749999999999994</v>
@@ -2137,10 +2141,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C13">
         <v>0.25</v>
@@ -2151,10 +2155,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C14">
         <v>0.3125</v>
@@ -2165,10 +2169,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>8.5714285714285701E-2</v>
@@ -2179,10 +2183,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <v>0.22857142857142856</v>
@@ -2193,10 +2197,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>0.22857142857142856</v>
@@ -2207,10 +2211,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C18">
         <v>0.22857142857142856</v>
@@ -2221,10 +2225,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C19">
         <v>0.22857142857142856</v>
@@ -2238,7 +2242,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C20">
         <v>5.2631578947368425E-2</v>
@@ -2252,7 +2256,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C21">
         <v>0.2105263157894737</v>
@@ -2266,7 +2270,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C22">
         <v>0.2105263157894737</v>
@@ -2280,7 +2284,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>0.10526315789473685</v>
@@ -2294,7 +2298,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C24">
         <v>0.4210526315789474</v>
@@ -2305,10 +2309,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>0.8</v>
@@ -2319,10 +2323,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C26">
         <v>0.2</v>
@@ -2333,10 +2337,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C27">
         <v>8.2644628099173556E-3</v>
@@ -2347,10 +2351,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C28">
         <v>8.2644628099173556E-2</v>
@@ -2361,10 +2365,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C29">
         <v>4.1322314049586778E-2</v>
@@ -2375,10 +2379,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C30">
         <v>0.24793388429752067</v>
@@ -2389,10 +2393,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C31">
         <v>0.57851239669421484</v>
@@ -2403,10 +2407,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>4.1322314049586778E-2</v>
@@ -2417,10 +2421,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C33">
         <v>0.11764705882352942</v>
@@ -2431,10 +2435,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C34">
         <v>0.11764705882352942</v>
@@ -2445,10 +2449,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C35">
         <v>0.29411764705882354</v>
@@ -2459,10 +2463,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C36">
         <v>0.23529411764705885</v>
@@ -2473,10 +2477,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C37">
         <v>0.11764705882352942</v>
@@ -2487,10 +2491,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C38">
         <v>0.11764705882352942</v>
@@ -2501,10 +2505,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C39">
         <v>0.15384615384615385</v>
@@ -2515,10 +2519,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C40">
         <v>0.11538461538461538</v>
@@ -2529,10 +2533,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C41">
         <v>0.30769230769230771</v>
@@ -2543,10 +2547,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C42">
         <v>0.11538461538461538</v>
@@ -2557,10 +2561,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C43">
         <v>0.30769230769230771</v>
@@ -2571,10 +2575,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C44">
         <v>0.13636363636363635</v>
@@ -2585,10 +2589,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C45">
         <v>0.13636363636363635</v>
@@ -2599,10 +2603,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C46">
         <v>4.5454545454545456E-2</v>
@@ -2613,10 +2617,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C47">
         <v>0.13636363636363635</v>
@@ -2627,10 +2631,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C48">
         <v>0.36363636363636365</v>
@@ -2641,10 +2645,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C49">
         <v>9.0909090909090912E-2</v>
@@ -2655,10 +2659,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C50">
         <v>9.0909090909090912E-2</v>
@@ -2669,10 +2673,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C51">
         <v>0.24242424242424246</v>
@@ -2683,10 +2687,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C52">
         <v>0.21212121212121213</v>
@@ -2697,10 +2701,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B53" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C53">
         <v>0.12121212121212123</v>
@@ -2711,10 +2715,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B54" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -2725,10 +2729,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B55" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C55">
         <v>0.21212121212121213</v>
@@ -2739,10 +2743,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C56">
         <v>0.21212121212121213</v>
@@ -2753,10 +2757,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C57">
         <v>0.3174603174603175</v>
@@ -2767,10 +2771,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C58">
         <v>9.5238095238095247E-2</v>
@@ -2781,10 +2785,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C59">
         <v>0.22222222222222224</v>
@@ -2795,10 +2799,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C60">
         <v>1.5873015873015876E-2</v>
@@ -2809,10 +2813,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C61">
         <v>9.5238095238095247E-2</v>
@@ -2823,10 +2827,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C62">
         <v>0.15873015873015875</v>
@@ -2837,10 +2841,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C63">
         <v>9.5238095238095247E-2</v>
@@ -2854,7 +2858,7 @@
         <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C64">
         <v>0.1</v>
@@ -2868,7 +2872,7 @@
         <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C65">
         <v>0.1</v>
@@ -2882,7 +2886,7 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C66">
         <v>0.125</v>
@@ -2896,7 +2900,7 @@
         <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C67">
         <v>0.125</v>
@@ -2910,7 +2914,7 @@
         <v>4</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C68">
         <v>0.2</v>
@@ -2924,7 +2928,7 @@
         <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C69">
         <v>0.17499999999999999</v>
@@ -2938,7 +2942,7 @@
         <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C70">
         <v>0.17499999999999999</v>
@@ -2968,24 +2972,24 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3002,7 +3006,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1">
         <v>0.21052631599999999</v>
@@ -3019,7 +3023,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1">
         <v>0.41666666699999999</v>
@@ -3036,7 +3040,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1">
         <v>0.485714286</v>
@@ -3053,7 +3057,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1">
         <v>0.22415575500000001</v>
@@ -3070,7 +3074,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1">
         <v>0.485714286</v>
@@ -3087,7 +3091,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1">
         <v>0.21052631599999999</v>
@@ -3104,7 +3108,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1">
         <v>0.157571773</v>
@@ -3121,7 +3125,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>0.27272727299999999</v>
@@ -3141,7 +3145,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1">
         <v>0.26666666700000002</v>
@@ -3161,7 +3165,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1">
         <v>0.31069958800000003</v>
@@ -3181,7 +3185,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1">
         <v>0.44892996099999999</v>
@@ -3198,7 +3202,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1">
         <v>0.41666666699999999</v>
@@ -3215,7 +3219,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1">
         <v>0.46875</v>
@@ -3232,7 +3236,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1">
         <v>0.21052631599999999</v>
@@ -3249,7 +3253,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>0.36363636399999999</v>
@@ -3266,7 +3270,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1">
         <v>0.4</v>
@@ -3296,6 +3300,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F00E7D3C5223B647BCF0704F4FD63FF8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="274554e3832af7cc9064f5d6743782b1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c3b4031e-841f-46f6-bede-a60d28c4ce79" xmlns:ns3="25f82bdf-59aa-449e-b461-28a7236b0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2c96c06903633a0219cb8332eecd029" ns2:_="" ns3:_="">
     <xsd:import namespace="c3b4031e-841f-46f6-bede-a60d28c4ce79"/>
@@ -3512,15 +3525,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23E7D15A-7770-4D3B-91AE-A46500598E63}">
   <ds:schemaRefs>
@@ -3539,6 +3543,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68A1C96F-6EFB-4028-BCE1-ECC515F0B18C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E8936A6-10D5-4CB1-A985-45E67CE71791}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3555,12 +3567,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68A1C96F-6EFB-4028-BCE1-ECC515F0B18C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update ui to have a "split" input for how to divide conditions to treatments
</commit_message>
<xml_diff>
--- a/params.xlsx
+++ b/params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.jemmett\dev\R\active_projects\723_mh_covid_surge_modelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433DA4D3-3B7A-4BE0-A531-9E24019BF7A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3231637B-CC7B-4914-B58A-319CDABC9257}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="3" xr2:uid="{F50B436A-7669-4109-9972-A64F78759D89}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="72">
   <si>
     <t>General population</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>Depression (Students)</t>
+  </si>
+  <si>
+    <t>split</t>
   </si>
 </sst>
 </file>
@@ -1966,7 +1969,8 @@
     <col min="1" max="1" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1977,7 +1981,7 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
         <v>47</v>
@@ -1991,7 +1995,7 @@
         <v>28</v>
       </c>
       <c r="C2">
-        <v>0.2</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>0.71</v>
@@ -2005,7 +2009,7 @@
         <v>30</v>
       </c>
       <c r="C3">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0.99</v>
@@ -2019,7 +2023,7 @@
         <v>29</v>
       </c>
       <c r="C4">
-        <v>0.6</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>0.91</v>
@@ -2033,7 +2037,7 @@
         <v>31</v>
       </c>
       <c r="C5">
-        <v>0.15</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>0.05</v>
@@ -2041,615 +2045,615 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.53</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C7">
-        <v>0.13513513513513514</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8">
-        <v>0.24324324324324326</v>
+        <v>12</v>
       </c>
       <c r="D8">
-        <v>0.71</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9">
-        <v>0.27027027027027029</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>0.99</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="C10">
-        <v>0.10810810810810811</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>0.84</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C11">
-        <v>0.24324324324324326</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0.91</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C12">
-        <v>0.25</v>
+        <v>14</v>
       </c>
       <c r="D12">
-        <v>0.71</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13">
-        <v>0.32812499999999994</v>
+        <v>24</v>
       </c>
       <c r="D13">
-        <v>0.84</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C14">
-        <v>0.1875</v>
+        <v>27</v>
       </c>
       <c r="D14">
-        <v>0.56999999999999995</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15">
-        <v>0.234375</v>
+        <v>11</v>
       </c>
       <c r="D15">
-        <v>0.05</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16">
-        <v>0.2</v>
+        <v>24</v>
       </c>
       <c r="D16">
-        <v>0.71</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C17">
-        <v>0.26249999999999996</v>
+        <v>14</v>
       </c>
       <c r="D17">
-        <v>0.84</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C18">
-        <v>0.15000000000000002</v>
+        <v>86</v>
       </c>
       <c r="D18">
-        <v>0.56999999999999995</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C19">
-        <v>0.1875</v>
+        <v>14</v>
       </c>
       <c r="D19">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C20">
-        <v>0.2</v>
+        <v>24</v>
       </c>
       <c r="D20">
-        <v>0.28999999999999998</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C21">
-        <v>0.25</v>
+        <v>27</v>
       </c>
       <c r="D21">
-        <v>0.71</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22">
-        <v>0.25</v>
+        <v>11</v>
       </c>
       <c r="D22">
-        <v>0.99</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="C23">
-        <v>0.25</v>
+        <v>24</v>
       </c>
       <c r="D23">
-        <v>0.84</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="D24">
-        <v>0.91</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C25">
-        <v>0.22222222222222224</v>
+        <v>33</v>
       </c>
       <c r="D25">
-        <v>0.71</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C26">
-        <v>0.22222222222222224</v>
+        <v>19</v>
       </c>
       <c r="D26">
-        <v>0.99</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C27">
-        <v>0.11111111111111112</v>
+        <v>23</v>
       </c>
       <c r="D27">
-        <v>0.84</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28">
-        <v>0.44444444444444448</v>
+        <v>16</v>
       </c>
       <c r="D28">
-        <v>0.91</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C29">
-        <v>0.8</v>
+        <v>21</v>
       </c>
       <c r="D29">
-        <v>0.05</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C30">
-        <v>0.2</v>
+        <v>12</v>
       </c>
       <c r="D30">
-        <v>0.05</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C31">
-        <v>8.2644628099173556E-3</v>
+        <v>15</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C32">
-        <v>8.2644628099173556E-2</v>
+        <v>16</v>
       </c>
       <c r="D32">
-        <v>0.71</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C33">
-        <v>4.1322314049586778E-2</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>0.84</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C34">
-        <v>0.24793388429752067</v>
+        <v>1</v>
       </c>
       <c r="D34">
-        <v>0.91</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35">
-        <v>0.57851239669421484</v>
+        <v>1</v>
       </c>
       <c r="D35">
-        <v>0.23</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C36">
-        <v>4.1322314049586778E-2</v>
+        <v>1</v>
       </c>
       <c r="D36">
-        <v>0.05</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C37">
-        <v>0.15384615384615385</v>
+        <v>20</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C38">
-        <v>0.11538461538461538</v>
+        <v>20</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C39">
-        <v>0.30769230769230771</v>
+        <v>10</v>
       </c>
       <c r="D39">
-        <v>0.47</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C40">
-        <v>0.11538461538461538</v>
+        <v>50</v>
       </c>
       <c r="D40">
-        <v>0.71</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C41">
-        <v>0.30769230769230771</v>
+        <v>4</v>
       </c>
       <c r="D41">
-        <v>0.91</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C42">
-        <v>0.13636363636363635</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C43">
-        <v>0.13636363636363635</v>
+        <v>1</v>
       </c>
       <c r="D43">
-        <v>0.71</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C44">
-        <v>4.5454545454545456E-2</v>
+        <v>8</v>
       </c>
       <c r="D44">
-        <v>0.84</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C45">
-        <v>0.13636363636363635</v>
+        <v>4</v>
       </c>
       <c r="D45">
-        <v>0.56999999999999995</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C46">
-        <v>0.36363636363636365</v>
+        <v>25</v>
       </c>
       <c r="D46">
-        <v>0.93</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C47">
-        <v>9.0909090909090912E-2</v>
+        <v>58</v>
       </c>
       <c r="D47">
-        <v>0.05</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C48">
-        <v>9.0909090909090912E-2</v>
+        <v>4</v>
       </c>
       <c r="D48">
-        <v>0.28999999999999998</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
         <v>40</v>
       </c>
       <c r="C49">
-        <v>0.30769230769230771</v>
+        <v>16</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -2657,251 +2661,251 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C50">
-        <v>0.26923076923076922</v>
+        <v>12</v>
       </c>
       <c r="D50">
-        <v>0.84</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C51">
-        <v>0.15384615384615385</v>
+        <v>30</v>
       </c>
       <c r="D51">
-        <v>0.91</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C52">
-        <v>0.26923076923076922</v>
+        <v>12</v>
       </c>
       <c r="D52">
-        <v>0.05</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C53">
-        <v>0.3174603174603175</v>
+        <v>30</v>
       </c>
       <c r="D53">
-        <v>0.47</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C54">
-        <v>9.5238095238095247E-2</v>
+        <v>15</v>
       </c>
       <c r="D54">
-        <v>0.71</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C55">
-        <v>0.22222222222222224</v>
+        <v>12</v>
       </c>
       <c r="D55">
-        <v>0.89</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="C56">
-        <v>1.5873015873015876E-2</v>
+        <v>73</v>
       </c>
       <c r="D56">
-        <v>0.99</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C57">
-        <v>9.5238095238095247E-2</v>
+        <v>14</v>
       </c>
       <c r="D57">
-        <v>0.84</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C58">
-        <v>0.15873015873015875</v>
+        <v>14</v>
       </c>
       <c r="D58">
-        <v>0.56999999999999995</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59">
         <v>5</v>
       </c>
-      <c r="B59" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59">
-        <v>9.5238095238095247E-2</v>
-      </c>
       <c r="D59">
-        <v>0.28999999999999998</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B60" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C60">
-        <v>0.1</v>
+        <v>14</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B61" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C61">
-        <v>0.22500000000000001</v>
+        <v>35</v>
       </c>
       <c r="D61">
-        <v>0.71</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C62">
-        <v>0.17499999999999999</v>
+        <v>9</v>
       </c>
       <c r="D62">
-        <v>0.84</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B63" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C63">
-        <v>0.2</v>
+        <v>9</v>
       </c>
       <c r="D63">
-        <v>0.93</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C64">
-        <v>0.22500000000000001</v>
+        <v>14</v>
       </c>
       <c r="D64">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="C65">
-        <v>7.4999999999999997E-2</v>
+        <v>50</v>
       </c>
       <c r="D65">
-        <v>0.28999999999999998</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D66">
-        <v>0.71</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B67" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C67">
-        <v>0.13513513513513514</v>
+        <v>30</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -2909,257 +2913,261 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B68" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="C68">
-        <v>0.86486486486486491</v>
+        <v>27</v>
       </c>
       <c r="D68">
-        <v>0.46</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B69" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C69">
-        <v>0.15384615384615385</v>
+        <v>16</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B70" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C70">
-        <v>0.11538461538461538</v>
+        <v>27</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B71" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="C71">
-        <v>0.73076923076923073</v>
+        <v>31</v>
       </c>
       <c r="D71">
-        <v>0.71</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="C72">
-        <v>0.13636363636363635</v>
+        <v>69</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="B73" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="C73">
-        <v>0.5</v>
+        <v>31</v>
       </c>
       <c r="D73">
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="B74" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C74">
-        <v>0.36363636363636365</v>
+        <v>8</v>
       </c>
       <c r="D74">
-        <v>0.93</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B75" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C75">
-        <v>0.30769230769230771</v>
+        <v>20</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B76" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C76">
-        <v>0.69230769230769229</v>
+        <v>9</v>
       </c>
       <c r="D76">
-        <v>0.46</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="B77" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="C77">
-        <v>0.2</v>
+        <v>9</v>
       </c>
       <c r="D77">
-        <v>0.71</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="B78" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C78">
-        <v>0.05</v>
+        <v>14</v>
       </c>
       <c r="D78">
-        <v>0.99</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="B79" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C79">
-        <v>0.6</v>
+        <v>9</v>
       </c>
       <c r="D79">
-        <v>0.91</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="B80" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C80">
-        <v>0.15</v>
+        <v>4</v>
       </c>
       <c r="D80">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C81">
-        <v>0.13513513513513514</v>
+        <v>9</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="C82">
-        <v>0.27027027027027029</v>
+        <v>7</v>
       </c>
       <c r="D82">
-        <v>0.71</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C83">
-        <v>0.27027027027027029</v>
+        <v>8</v>
       </c>
       <c r="D83">
-        <v>0.99</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C84">
-        <v>0.10810810810810811</v>
+        <v>9</v>
       </c>
       <c r="D84">
-        <v>0.84</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C85">
-        <v>0.21621621621621623</v>
+        <v>3</v>
       </c>
       <c r="D85">
-        <v>0.91</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D85">
+    <sortCondition ref="A2:A85"/>
+    <sortCondition ref="B2:B85"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>